<commit_message>
open ai code implementation
</commit_message>
<xml_diff>
--- a/OpenAI Classification/Articles_to_Score_Complete.xlsx
+++ b/OpenAI Classification/Articles_to_Score_Complete.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/5da7b48e0d9e2372/Documents/BSE/Term 3/Masters Thesis/ECB_Perceived_Cacophony/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\monbi\OneDrive\Documents\BSE\Term 3\Masters Thesis\ECB_Perceived_Cacophony\OpenAI Classification\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="14_{8F904859-5603-490B-B4DE-F084B30093EC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F837283F-0CDD-4272-BB4D-ACAD5CE7D6C8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{2F547B85-2458-42BE-B5B3-987A19E09DC2}"/>
   </bookViews>
@@ -360,7 +360,7 @@
     <t>The prices of German Bunds rose on 3 March. The market attributed the price gains to a countermovement to the losses on 2 March. In the euro area, the high inflationary pressure at the corporate level weakened significantly at the beginning of the year. While overall inflation fell slightly in February, core inflation rose to a record high. Economists interpret this as an indication that price pressures from the energy and commodities sectors could spread to other sectors, such as services. The  ECB  is, therefore, likely to raise its interest rates again by 0.50 percentage points in mid-March. Several  central bankers  argued that further rate hikes were necessary to curb high inflation.  ECB  Vice-President  Luis de Guindos  emphasised the importance of underlying inflation.</t>
   </si>
   <si>
-    <t>Classificaton Ed</t>
+    <t>Classification Ed</t>
   </si>
 </sst>
 </file>
@@ -428,6 +428,10 @@
 </styleSheet>
 </file>
 
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
+</file>
+
 <file path=xl/queryTables/queryTable1.xml><?xml version="1.0" encoding="utf-8"?>
 <queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="ExternalData_1" connectionId="1" xr16:uid="{D26C9A31-6325-4894-9BA1-FAEEDF0D207F}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0">
   <queryTableRefresh nextId="7" unboundColumnsRight="1">
@@ -453,7 +457,7 @@
     <tableColumn id="2" xr3:uid="{657E8E3A-F917-45D3-95EC-5AF6670649D2}" uniqueName="2" name="Manual.summary" queryTableFieldId="2" dataDxfId="3"/>
     <tableColumn id="3" xr3:uid="{95E71AAD-BAAE-49E5-BF00-B0800BBD5EFD}" uniqueName="3" name="Classification Joaquin" queryTableFieldId="3" dataDxfId="2"/>
     <tableColumn id="4" xr3:uid="{EA4A99FC-D149-4362-8F40-D3A24C070DE9}" uniqueName="4" name="Classification Rui" queryTableFieldId="4" dataDxfId="1"/>
-    <tableColumn id="5" xr3:uid="{C1E7B947-EB0F-468E-8635-8AF655CBE387}" uniqueName="5" name="Classificaton Ed" queryTableFieldId="6" dataDxfId="0"/>
+    <tableColumn id="5" xr3:uid="{C1E7B947-EB0F-468E-8635-8AF655CBE387}" uniqueName="5" name="Classification Ed" queryTableFieldId="6" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -778,8 +782,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{02D15B92-11E3-4CB8-90DE-1897D037A5D2}">
   <dimension ref="A1:E101"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -788,7 +792,7 @@
     <col min="2" max="2" width="164.5546875" customWidth="1"/>
     <col min="3" max="3" width="23.33203125" customWidth="1"/>
     <col min="4" max="4" width="19.33203125" customWidth="1"/>
-    <col min="5" max="5" width="16.6640625" customWidth="1"/>
+    <col min="5" max="5" width="25.33203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.3">

</xml_diff>